<commit_message>
Fleshing out the Weapons and Shield classes.
Added Result class.
Added WeaponType class
Added Logic
</commit_message>
<xml_diff>
--- a/Documentation/weapons_and_shields.xlsx
+++ b/Documentation/weapons_and_shields.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="19095" windowHeight="12000"/>
-    <workbookView xWindow="19305" yWindow="60" windowWidth="19020" windowHeight="11895" activeTab="1"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="11328" windowHeight="4728" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
     <sheet name="Shields" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -178,8 +177,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +379,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -414,6 +414,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,29 +590,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="7" width="25.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -637,7 +637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -665,7 +665,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -721,7 +721,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -749,7 +749,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -777,7 +777,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -805,7 +805,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -833,7 +833,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -861,7 +861,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -889,7 +889,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -917,7 +917,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -945,7 +945,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -973,7 +973,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1235,30 +1235,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="1">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1340,7 +1339,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1368,7 +1367,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1396,7 +1395,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1424,7 +1423,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1452,7 +1451,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1480,7 +1479,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1508,7 +1507,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
@@ -1536,7 +1535,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -1564,7 +1563,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
@@ -1592,7 +1591,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>51</v>
       </c>
@@ -1630,13 +1629,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>